<commit_message>
Add UpdateFormulas script and enhance OH_Refacturacion logic for Folio formatting
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://repsol365-my.sharepoint.com/personal/manuel_villanueva_servexternos_repsol_com/Documents/Documentos/UiPath/Reporte-Regulatorio_Refacturacion/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{6F4E8EB0-9CD1-4FE3-A9AB-79E93993D805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E305AFE0-8507-41C4-A725-FE9646943F0A}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{6F4E8EB0-9CD1-4FE3-A9AB-79E93993D805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293BB571-53FE-4742-99AB-56072506CAA8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +336,81 @@
   </si>
   <si>
     <t>C:\ReporteRegulatorioRpa\Output\XML</t>
+  </si>
+  <si>
+    <t>DateRefacturacion</t>
+  </si>
+  <si>
+    <t>Emonth</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -388,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,6 +476,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,9 +795,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z972"/>
+  <dimension ref="A1:Z974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -826,201 +902,219 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f ca="1">VLOOKUP(B4,Meses!A:C,3,FALSE)</f>
+        <v>Jun</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="6" t="str">
+      <c r="B8" s="6" t="str">
         <f ca="1">_xlfn.CONCAT(B6," ",B3)</f>
         <v>junio 2025</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f ca="1">_xlfn.CONCAT(B7," ",B3)</f>
+        <v>Jun 2025</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="str">
-        <f>_xlfn.CONCAT(B8,"Input\")</f>
-        <v>C:\ReporteRegulatorioRpa\Input\</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="str">
-        <f>_xlfn.CONCAT(B8,"Output\")</f>
-        <v>C:\ReporteRegulatorioRpa\Output\</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" t="str">
-        <f>_xlfn.CONCAT(B8,"Temp\")</f>
-        <v>C:\ReporteRegulatorioRpa\Temp\</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
+        <f>_xlfn.CONCAT(B10,"Input\")</f>
+        <v>C:\ReporteRegulatorioRpa\Input\</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B12" t="str">
-        <f>_xlfn.CONCAT(B11,"REXM - Overhead facturable MMyyyya",".xlsx")</f>
-        <v>C:\ReporteRegulatorioRpa\Temp\REXM - Overhead facturable MMyyyya.xlsx</v>
+        <f>_xlfn.CONCAT(B10,"Output\")</f>
+        <v>C:\ReporteRegulatorioRpa\Output\</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>88</v>
+      <c r="A13" t="s">
+        <v>16</v>
       </c>
       <c r="B13" t="str">
-        <f>_xlfn.CONCAT(B11,"Refacturacion_regular_v2.xlsm")</f>
-        <v>C:\ReporteRegulatorioRpa\Temp\Refacturacion_regular_v2.xlsm</v>
-      </c>
-      <c r="C13" s="4"/>
+        <f>_xlfn.CONCAT(B10,"Temp\")</f>
+        <v>C:\ReporteRegulatorioRpa\Temp\</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B9,"Refacturacion_regular_v2 ",B7,".xlsm")</f>
-        <v>C:\ReporteRegulatorioRpa\Input\Refacturacion_regular_v2 junio 2025.xlsm</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B14" t="str">
+        <f>_xlfn.CONCAT(B13,"REXM - Overhead facturable MMyyyya",".xlsx")</f>
+        <v>C:\ReporteRegulatorioRpa\Temp\REXM - Overhead facturable MMyyyya.xlsx</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="B15" t="str">
+        <f>_xlfn.CONCAT(B13,"Refacturacion_regular_v2.xlsm")</f>
+        <v>C:\ReporteRegulatorioRpa\Temp\Refacturacion_regular_v2.xlsm</v>
       </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" t="str">
-        <f ca="1">_xlfn.CONCAT("Layout refacturación ",$B$7,".xlsx")</f>
-        <v>Layout refacturación junio 2025.xlsx</v>
+        <v>93</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(B11,"Refacturacion_regular_v2 ",B8,".xlsm")</f>
+        <v>C:\ReporteRegulatorioRpa\Input\Refacturacion_regular_v2 junio 2025.xlsm</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" t="str">
-        <f ca="1">_xlfn.CONCAT("Layout refacturación_NC ",$B$7,".xlsx")</f>
-        <v>Layout refacturación_NC junio 2025.xlsx</v>
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B18" t="str">
-        <f ca="1">_xlfn.CONCAT("REXM - Overhead facturable ",B7,".xlsx")</f>
-        <v>REXM - Overhead facturable junio 2025.xlsx</v>
+        <f ca="1">_xlfn.CONCAT("Layout refacturación ",$B$8,".xlsx")</f>
+        <v>Layout refacturación junio 2025.xlsx</v>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
+        <v>95</v>
+      </c>
+      <c r="B19" t="str">
+        <f ca="1">_xlfn.CONCAT("Layout refacturación_NC ",$B$8,".xlsx")</f>
+        <v>Layout refacturación_NC junio 2025.xlsx</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B20" t="str">
-        <f>_xlfn.CONCAT(B11,"Layout refacturación",".xlsx")</f>
-        <v>C:\ReporteRegulatorioRpa\Temp\Layout refacturación.xlsx</v>
+        <f ca="1">_xlfn.CONCAT("REXM - Overhead facturable ",B8,".xlsx")</f>
+        <v>REXM - Overhead facturable junio 2025.xlsx</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" t="str">
-        <f ca="1">_xlfn.CONCAT(B9,"REXMEX - Cuenta Operativa ",B5,B3,".xlsx")</f>
-        <v>C:\ReporteRegulatorioRpa\Input\REXMEX - Cuenta Operativa 062025.xlsx</v>
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
+        <v>72</v>
+      </c>
+      <c r="B22" t="str">
+        <f>_xlfn.CONCAT(B13,"Layout refacturación",".xlsx")</f>
+        <v>C:\ReporteRegulatorioRpa\Temp\Layout refacturación.xlsx</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="str">
+        <f ca="1">_xlfn.CONCAT(B11,"REXMEX - Cuenta Operativa ",B5,B3,".xlsx")</f>
+        <v>C:\ReporteRegulatorioRpa\Input\REXMEX - Cuenta Operativa 062025.xlsx</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B27" s="6">
         <v>3</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1966,6 +2060,8 @@
     <row r="970" ht="14.25" customHeight="1"/>
     <row r="971" ht="14.25" customHeight="1"/>
     <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4223,116 +4319,155 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46765C1-F135-4C0B-8C59-9A5E5B810784}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2">
-        <v>6</v>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2">
-        <v>7</v>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2">
-        <v>8</v>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2">
-        <v>9</v>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2">
-        <v>10</v>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2">
-        <v>11</v>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2">
-        <v>12</v>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>